<commit_message>
feat: 29-10-25 v2 version
</commit_message>
<xml_diff>
--- a/TRAMAS/EJEMPLO ASIGNACION.xlsx
+++ b/TRAMAS/EJEMPLO ASIGNACION.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chizo\Music\cashi\web-app-cashi\TRAMAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\contacto-total\cashi\TRAMAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6F92EB-5AE7-4605-872D-6AF99DF40CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D059B85-AEC0-433C-961A-D08BF68581F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="105" windowWidth="18750" windowHeight="15495" xr2:uid="{F2385CA5-23F7-42A7-A31A-37C2506AA8EC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F2385CA5-23F7-42A7-A31A-37C2506AA8EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="127">
   <si>
     <t>PERIODO</t>
   </si>
@@ -259,6 +259,162 @@
   </si>
   <si>
     <t>VILLA EL SALVADOR</t>
+  </si>
+  <si>
+    <t>D000006860887</t>
+  </si>
+  <si>
+    <t>4040710025570837</t>
+  </si>
+  <si>
+    <t>HECTOR FELICIANO DONGO CERVANTES</t>
+  </si>
+  <si>
+    <t>HECTOR</t>
+  </si>
+  <si>
+    <t>DONGO</t>
+  </si>
+  <si>
+    <t>hectordongo@hotmail.com</t>
+  </si>
+  <si>
+    <t>AVENIDA CASANAVE NRO. 477 EL CARMEN</t>
+  </si>
+  <si>
+    <t>COMAS</t>
+  </si>
+  <si>
+    <t>D000075339664</t>
+  </si>
+  <si>
+    <t>4040710009376979</t>
+  </si>
+  <si>
+    <t>ADEMIR ORESTES BURNES MEZA</t>
+  </si>
+  <si>
+    <t>ADEMIR</t>
+  </si>
+  <si>
+    <t>BURNES</t>
+  </si>
+  <si>
+    <t>aderdark1@gmail.com</t>
+  </si>
+  <si>
+    <t>C NRO. 23 ASENT. HUMANO INDEPENDENCIA</t>
+  </si>
+  <si>
+    <t>NUEVO CHIMBOTE</t>
+  </si>
+  <si>
+    <t>ANCASH</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>D000040212926</t>
+  </si>
+  <si>
+    <t>5339580005090503</t>
+  </si>
+  <si>
+    <t>BETTY LILIANA GUTIERREZ TAPIA</t>
+  </si>
+  <si>
+    <t>BETTY</t>
+  </si>
+  <si>
+    <t>GUTIERREZ</t>
+  </si>
+  <si>
+    <t>bettylilianagutuerreztapia@gmail.com.com</t>
+  </si>
+  <si>
+    <t>CALLE MANUEL GONZALES PRADA MZ J LOTE 20 NRO. 1</t>
+  </si>
+  <si>
+    <t>FERREÑAFE</t>
+  </si>
+  <si>
+    <t>LAMBAYEQUE</t>
+  </si>
+  <si>
+    <t>D000018124448</t>
+  </si>
+  <si>
+    <t>4040710025533918</t>
+  </si>
+  <si>
+    <t>ABRAHAM JOSE TIRADO CORTEZ</t>
+  </si>
+  <si>
+    <t>ABRAHAM</t>
+  </si>
+  <si>
+    <t>TIRADO</t>
+  </si>
+  <si>
+    <t>abrahamtiradocortez@gmail.com</t>
+  </si>
+  <si>
+    <t>A4 LOT 24 II ETAPA MANUEL AREVALO</t>
+  </si>
+  <si>
+    <t>LA ESPERANZA</t>
+  </si>
+  <si>
+    <t>D000043039736</t>
+  </si>
+  <si>
+    <t>4040710024635342</t>
+  </si>
+  <si>
+    <t>JOSUE SALAZAR FERNANDEZ</t>
+  </si>
+  <si>
+    <t>JOSUE</t>
+  </si>
+  <si>
+    <t>SALAZAR</t>
+  </si>
+  <si>
+    <t>salazarfernandezjosue17@gmail.com</t>
+  </si>
+  <si>
+    <t>AVENIDA ZONA B      C</t>
+  </si>
+  <si>
+    <t>ATE</t>
+  </si>
+  <si>
+    <t>D000041317332</t>
+  </si>
+  <si>
+    <t>5246010006688644</t>
+  </si>
+  <si>
+    <t>HELMER RAUL SALAS CALVO</t>
+  </si>
+  <si>
+    <t>HELMER</t>
+  </si>
+  <si>
+    <t>SALAS</t>
+  </si>
+  <si>
+    <t>hsc40@hotmail.com</t>
+  </si>
+  <si>
+    <t>CALLE LEON VELARDE NRO. 104 EDIFICIO CASA 20 URBANIZACION QUINTA SANTA EUGENIA</t>
+  </si>
+  <si>
+    <t>YANAHUARA</t>
+  </si>
+  <si>
+    <t>AREQUIPA</t>
   </si>
 </sst>
 </file>
@@ -329,9 +485,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -369,7 +525,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -475,7 +631,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -617,7 +773,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -625,21 +781,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31854E9-73E7-49AE-B0ED-6E38A4438237}">
-  <dimension ref="A1:AF5"/>
+  <dimension ref="A1:AF11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" ht="15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -737,7 +890,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>202510</v>
       </c>
@@ -760,7 +913,7 @@
         <v>36</v>
       </c>
       <c r="H2" s="4">
-        <v>1310.04</v>
+        <v>3101.04</v>
       </c>
       <c r="I2">
         <v>19589.580000000002</v>
@@ -796,7 +949,7 @@
         <v>40</v>
       </c>
       <c r="T2">
-        <v>949356887</v>
+        <v>1001</v>
       </c>
       <c r="U2">
         <v>255983</v>
@@ -835,7 +988,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>202510</v>
       </c>
@@ -858,7 +1011,7 @@
         <v>50</v>
       </c>
       <c r="H3" s="4">
-        <v>500.1</v>
+        <v>3105.04</v>
       </c>
       <c r="I3">
         <v>46949.35</v>
@@ -894,7 +1047,7 @@
         <v>53</v>
       </c>
       <c r="T3">
-        <v>989869161</v>
+        <v>1002</v>
       </c>
       <c r="W3">
         <v>4744087</v>
@@ -927,7 +1080,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>202510</v>
       </c>
@@ -986,7 +1139,7 @@
         <v>62</v>
       </c>
       <c r="T4">
-        <v>992240649</v>
+        <v>1003</v>
       </c>
       <c r="W4">
         <v>989751851</v>
@@ -1019,7 +1172,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>202510</v>
       </c>
@@ -1078,7 +1231,7 @@
         <v>71</v>
       </c>
       <c r="T5">
-        <v>998835274</v>
+        <v>1004</v>
       </c>
       <c r="U5">
         <v>2933338</v>
@@ -1111,6 +1264,549 @@
         <v>6902</v>
       </c>
       <c r="AF5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>202510</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6">
+        <v>67</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="4">
+        <v>7419.1</v>
+      </c>
+      <c r="I6">
+        <v>34454.639999999999</v>
+      </c>
+      <c r="J6">
+        <v>40034.26</v>
+      </c>
+      <c r="K6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6">
+        <v>66</v>
+      </c>
+      <c r="M6" s="4">
+        <v>7419.1</v>
+      </c>
+      <c r="N6">
+        <v>34454.639999999999</v>
+      </c>
+      <c r="O6">
+        <v>40034.26</v>
+      </c>
+      <c r="P6" s="5">
+        <v>45955</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>77</v>
+      </c>
+      <c r="R6" t="s">
+        <v>78</v>
+      </c>
+      <c r="S6" t="s">
+        <v>79</v>
+      </c>
+      <c r="T6">
+        <v>1005</v>
+      </c>
+      <c r="V6">
+        <v>3154000</v>
+      </c>
+      <c r="W6">
+        <v>3693989</v>
+      </c>
+      <c r="X6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y6">
+        <v>60</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE6">
+        <v>27574</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>202510</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7">
+        <v>77</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1748.53</v>
+      </c>
+      <c r="I7">
+        <v>2860.06</v>
+      </c>
+      <c r="J7">
+        <v>3402.97</v>
+      </c>
+      <c r="K7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7">
+        <v>76</v>
+      </c>
+      <c r="M7" s="4">
+        <v>1748.53</v>
+      </c>
+      <c r="N7">
+        <v>2860.06</v>
+      </c>
+      <c r="O7">
+        <v>3402.97</v>
+      </c>
+      <c r="P7" s="5">
+        <v>45945</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>85</v>
+      </c>
+      <c r="R7" t="s">
+        <v>86</v>
+      </c>
+      <c r="S7" t="s">
+        <v>87</v>
+      </c>
+      <c r="T7">
+        <v>1006</v>
+      </c>
+      <c r="W7">
+        <v>943831359</v>
+      </c>
+      <c r="X7">
+        <v>933970220</v>
+      </c>
+      <c r="Y7">
+        <v>28</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE7">
+        <v>2585</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>202510</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8">
+        <v>77</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="4">
+        <v>231.83</v>
+      </c>
+      <c r="I8">
+        <v>427.11</v>
+      </c>
+      <c r="J8">
+        <v>580.28</v>
+      </c>
+      <c r="K8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8">
+        <v>76</v>
+      </c>
+      <c r="M8" s="4">
+        <v>231.83</v>
+      </c>
+      <c r="N8">
+        <v>427.11</v>
+      </c>
+      <c r="O8">
+        <v>580.28</v>
+      </c>
+      <c r="P8" s="5">
+        <v>45945</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>95</v>
+      </c>
+      <c r="R8" t="s">
+        <v>96</v>
+      </c>
+      <c r="S8" t="s">
+        <v>97</v>
+      </c>
+      <c r="T8">
+        <v>1007</v>
+      </c>
+      <c r="Y8">
+        <v>46</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>98</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>202510</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9">
+        <v>87</v>
+      </c>
+      <c r="G9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="4">
+        <v>2274.71</v>
+      </c>
+      <c r="I9">
+        <v>6277.18</v>
+      </c>
+      <c r="J9">
+        <v>7242.25</v>
+      </c>
+      <c r="K9" t="s">
+        <v>37</v>
+      </c>
+      <c r="L9">
+        <v>86</v>
+      </c>
+      <c r="M9" s="4">
+        <v>2274.71</v>
+      </c>
+      <c r="N9">
+        <v>6277.18</v>
+      </c>
+      <c r="O9">
+        <v>7242.25</v>
+      </c>
+      <c r="P9" s="5">
+        <v>45935</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>104</v>
+      </c>
+      <c r="R9" t="s">
+        <v>105</v>
+      </c>
+      <c r="S9" t="s">
+        <v>106</v>
+      </c>
+      <c r="T9">
+        <v>1008</v>
+      </c>
+      <c r="Y9">
+        <v>53</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE9">
+        <v>5346</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>202510</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10">
+        <v>87</v>
+      </c>
+      <c r="G10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="4">
+        <v>560.04999999999995</v>
+      </c>
+      <c r="I10">
+        <v>442.55</v>
+      </c>
+      <c r="J10">
+        <v>595.01</v>
+      </c>
+      <c r="K10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10">
+        <v>86</v>
+      </c>
+      <c r="M10" s="4">
+        <v>560.04999999999995</v>
+      </c>
+      <c r="N10">
+        <v>442.55</v>
+      </c>
+      <c r="O10">
+        <v>595.01</v>
+      </c>
+      <c r="P10" s="5">
+        <v>45935</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>112</v>
+      </c>
+      <c r="R10" t="s">
+        <v>113</v>
+      </c>
+      <c r="S10" t="s">
+        <v>114</v>
+      </c>
+      <c r="T10">
+        <v>1009</v>
+      </c>
+      <c r="W10">
+        <v>995303541</v>
+      </c>
+      <c r="X10">
+        <v>980338832</v>
+      </c>
+      <c r="Y10">
+        <v>41</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>202510</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F11">
+        <v>138</v>
+      </c>
+      <c r="G11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="4">
+        <v>7591.85</v>
+      </c>
+      <c r="I11">
+        <v>52475</v>
+      </c>
+      <c r="J11">
+        <v>57774.35</v>
+      </c>
+      <c r="K11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11">
+        <v>137</v>
+      </c>
+      <c r="M11" s="4">
+        <v>7591.85</v>
+      </c>
+      <c r="N11">
+        <v>52475</v>
+      </c>
+      <c r="O11">
+        <v>57774.35</v>
+      </c>
+      <c r="P11" s="5">
+        <v>45945</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>120</v>
+      </c>
+      <c r="R11" t="s">
+        <v>121</v>
+      </c>
+      <c r="S11" t="s">
+        <v>122</v>
+      </c>
+      <c r="T11">
+        <v>1010</v>
+      </c>
+      <c r="U11">
+        <v>250180</v>
+      </c>
+      <c r="V11">
+        <v>247045</v>
+      </c>
+      <c r="W11">
+        <v>989400333</v>
+      </c>
+      <c r="X11" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y11">
+        <v>43</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>124</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE11">
+        <v>34119</v>
+      </c>
+      <c r="AF11" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>